<commit_message>
Last changes to hail_bom
</commit_message>
<xml_diff>
--- a/rev_a/hail_bom.xlsx
+++ b/rev_a/hail_bom.xlsx
@@ -798,8 +798,8 @@
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>